<commit_message>
Refined the boundaries of secondary correction
</commit_message>
<xml_diff>
--- a/rpm_acel_decel_time_corrected.xlsx
+++ b/rpm_acel_decel_time_corrected.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tan\Documents\Github\TMC2240_ESP32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2709E9F0-8EF7-4E9F-A662-8FBEE4D6D00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B425879-3F5B-491A-9CEB-0BF127C74F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -893,6 +893,41 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>&lt;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 700 RPM</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1310,6 +1345,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>&gt; 700 RPM</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3483,16 +3543,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>292344</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>71071</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>394138</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>26276</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>462329</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>90121</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>173295</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>162380</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3520,15 +3580,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>348030</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>20515</xdr:rowOff>
+      <xdr:colOff>131254</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>73067</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>389282</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>149087</xdr:rowOff>
+      <xdr:colOff>172506</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>11139</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3879,8 +3939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="S46" sqref="S46"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>